<commit_message>
Add another example to project
</commit_message>
<xml_diff>
--- a/src/example/my_grid.xlsx
+++ b/src/example/my_grid.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Path</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>.*.txt</t>
+  </si>
+  <si>
+    <t>watching aswell</t>
   </si>
 </sst>
 </file>
@@ -372,7 +375,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -398,6 +401,14 @@
         <v>3</v>
       </c>
     </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>